<commit_message>
Hoan tat Import den Applicant
</commit_message>
<xml_diff>
--- a/BTS.Web/ImportData/Mau ho so kiem dnh BTS.xlsx
+++ b/BTS.Web/ImportData/Mau ho so kiem dnh BTS.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="683" activeTab="7"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950" tabRatio="683"/>
   </bookViews>
   <sheets>
     <sheet name="InCaseOf" sheetId="11" r:id="rId1"/>
     <sheet name="Lab" sheetId="13" r:id="rId2"/>
     <sheet name="City" sheetId="10" r:id="rId3"/>
     <sheet name="Operator" sheetId="6" r:id="rId4"/>
-    <sheet name="Application" sheetId="7" r:id="rId5"/>
+    <sheet name="Applicant" sheetId="7" r:id="rId5"/>
     <sheet name="1_Profile" sheetId="8" r:id="rId6"/>
     <sheet name="1_BTS" sheetId="9" r:id="rId7"/>
     <sheet name="2_Certificate" sheetId="12" r:id="rId8"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="115">
   <si>
     <t>No</t>
   </si>
@@ -359,6 +359,27 @@
   </si>
   <si>
     <t>ContactName</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t>Hùng</t>
+  </si>
+  <si>
+    <t>VCC3</t>
+  </si>
+  <si>
+    <t>Trung tâm Kiểm định và Chứng nhận 3</t>
+  </si>
+  <si>
+    <t>42 Trần Quốc Toản, Đà Nẵng</t>
+  </si>
+  <si>
+    <t>VCC1</t>
+  </si>
+  <si>
+    <t>Trung tâm Kiểm định và Chứng nhận 1</t>
   </si>
 </sst>
 </file>
@@ -2225,8 +2246,8 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2301,10 +2322,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2362,15 +2383,25 @@
       <c r="A3" s="6">
         <v>2</v>
       </c>
+      <c r="B3" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="33" customHeight="1">
       <c r="A4" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="33" customHeight="1">
-      <c r="A5" s="6">
-        <v>4</v>
+      <c r="B4" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2663,7 +2694,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2802,6 +2833,18 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="5">
+        <v>2343253</v>
+      </c>
+      <c r="F2" s="5">
+        <v>5435345</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>24</v>
@@ -2895,7 +2938,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Application!$B$2:$B$20</xm:f>
+            <xm:f>Applicant!$B$2:$B$20</xm:f>
           </x14:formula1>
           <xm:sqref>A1:A1048576</xm:sqref>
         </x14:dataValidation>
@@ -2998,7 +3041,7 @@
   </sheetPr>
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G8" sqref="G7:G8"/>
     </sheetView>
   </sheetViews>
@@ -3127,7 +3170,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lab!$B$2:$B$20</xm:f>
+            <xm:f>Lab!$B$2:$B$18</xm:f>
           </x14:formula1>
           <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>

</xml_diff>